<commit_message>
Latest re-runs from Will
</commit_message>
<xml_diff>
--- a/Consequence_Table/BoRVOI_IBMR_final__results_v2.xlsx
+++ b/Consequence_Table/BoRVOI_IBMR_final__results_v2.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/bmahardja_usbr_gov/Documents/Documents/GitHub/DeltaSmelt_SummerFallX2_VOI/Consequence_Table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07ED0011-D4FF-487D-A55F-74F317316307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{07ED0011-D4FF-487D-A55F-74F317316307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{532B2816-E096-4BF6-96AD-EC3D637EB47D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F8F4939-3C7D-4924-953A-51F1997FE89C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{9F8F4939-3C7D-4924-953A-51F1997FE89C}"/>
   </bookViews>
   <sheets>
     <sheet name="IBMRv1" sheetId="1" r:id="rId1"/>
     <sheet name="IBMRv2" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="25">
   <si>
     <t>S74</t>
   </si>
@@ -119,6 +123,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,10 +161,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,7 +267,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>IBMRv1!$A$35</c:f>
+              <c:f>IBMRv1!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -271,7 +288,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>IBMRv1!$B$34:$F$34</c:f>
+              <c:f>IBMRv1!$B$32:$F$32</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -294,7 +311,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>IBMRv1!$B$35:$F$35</c:f>
+              <c:f>IBMRv1!$B$33:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -327,7 +344,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>IBMRv1!$A$36</c:f>
+              <c:f>IBMRv1!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -348,7 +365,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>IBMRv1!$B$34:$F$34</c:f>
+              <c:f>IBMRv1!$B$32:$F$32</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -371,7 +388,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>IBMRv1!$B$36:$F$36</c:f>
+              <c:f>IBMRv1!$B$34:$F$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -404,7 +421,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>IBMRv1!$A$37</c:f>
+              <c:f>IBMRv1!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -425,7 +442,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>IBMRv1!$B$34:$F$34</c:f>
+              <c:f>IBMRv1!$B$32:$F$32</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -448,7 +465,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>IBMRv1!$B$37:$F$37</c:f>
+              <c:f>IBMRv1!$B$35:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -481,7 +498,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>IBMRv1!$A$38</c:f>
+              <c:f>IBMRv1!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -502,7 +519,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>IBMRv1!$B$34:$F$34</c:f>
+              <c:f>IBMRv1!$B$32:$F$32</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -525,7 +542,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>IBMRv1!$B$38:$F$38</c:f>
+              <c:f>IBMRv1!$B$36:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2411,13 +2428,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>308610</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>62865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>62865</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2487,6 +2504,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2786,15 +2807,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931B29C3-DFB1-4324-838D-20404E986B8C}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U2" sqref="B2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -2807,7 +2830,7 @@
       <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2860,19 +2883,19 @@
       <c r="P2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2925,19 +2948,19 @@
       <c r="P3">
         <v>1.92088644293433</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="5">
         <v>1.3848354492328201</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="5">
         <v>1.3705134948937701</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="5">
         <v>1.4573011071575599</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="5">
         <v>1.1874398352853801</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="5">
         <v>1.55720574713289</v>
       </c>
     </row>
@@ -2990,19 +3013,19 @@
       <c r="P4">
         <v>0.81841070084330803</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="5">
         <v>0.92690913929374597</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="5">
         <v>0.76163754369259995</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="5">
         <v>0.79625233588664801</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="5">
         <v>0.81540161971796998</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="5">
         <v>0.96497745950410896</v>
       </c>
     </row>
@@ -3055,19 +3078,19 @@
       <c r="P5">
         <v>1.31496982793713</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="5">
         <v>1.2527565679571799</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="5">
         <v>1.2106716837257001</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="5">
         <v>1.2622225314437301</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="5">
         <v>1.13655672791882</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="5">
         <v>1.4637677274206999</v>
       </c>
     </row>
@@ -3120,19 +3143,19 @@
       <c r="P6">
         <v>2.0133309669324002</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="5">
         <v>1.97571508014206</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="5">
         <v>1.88803591425286</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="5">
         <v>1.9748174364828699</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="5">
         <v>1.8596117110713599</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="5">
         <v>1.99184463992009</v>
       </c>
     </row>
@@ -3185,19 +3208,19 @@
       <c r="P7">
         <v>1.5052857131797801</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="5">
         <v>2.1022366223836002</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="5">
         <v>1.7134695600932099</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="5">
         <v>1.72055050994479</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="5">
         <v>1.96060794868347</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="5">
         <v>1.9918298836199699</v>
       </c>
     </row>
@@ -3250,19 +3273,19 @@
       <c r="P8">
         <v>0.73241583381092001</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="5">
         <v>1.61277964310987</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="5">
         <v>1.43852787758232</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="5">
         <v>1.31147580950653</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="5">
         <v>1.4457672704255999</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="5">
         <v>1.5502000553497299</v>
       </c>
     </row>
@@ -3315,19 +3338,19 @@
       <c r="P9">
         <v>0.73774329369150404</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="5">
         <v>1.6473232763994501</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="5">
         <v>1.60507624632964</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="5">
         <v>1.6014358290394699</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="5">
         <v>1.6097578685879399</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="5">
         <v>1.6152134990057501</v>
       </c>
     </row>
@@ -3380,19 +3403,19 @@
       <c r="P10">
         <v>1.2191971528088901</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="5">
         <v>1.83548395685907</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="5">
         <v>1.87320618493937</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="5">
         <v>1.85105907325036</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="5">
         <v>1.7885391520195499</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="5">
         <v>1.83792756280946</v>
       </c>
     </row>
@@ -3445,19 +3468,19 @@
       <c r="P11">
         <v>0.56251849315068503</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="5">
         <v>1.00887762701273</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="5">
         <v>0.87049371331632197</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="5">
         <v>0.90587223910363601</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="5">
         <v>0.85723331503529898</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="5">
         <v>1.0301540426406099</v>
       </c>
     </row>
@@ -3510,19 +3533,19 @@
       <c r="P12">
         <v>0.65736289869522502</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="5">
         <v>0.62961080586080598</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="5">
         <v>0.698763204748728</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="5">
         <v>0.65917208439568498</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="5">
         <v>0.68358726084138199</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="5">
         <v>0.63149729344437799</v>
       </c>
     </row>
@@ -3575,19 +3598,19 @@
       <c r="P13">
         <v>0.85753857321858196</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="5">
         <v>0.94569064874277298</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="5">
         <v>0.98322709224706495</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="5">
         <v>0.996672241844066</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="5">
         <v>0.96791781017011902</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="5">
         <v>0.99530116892346598</v>
       </c>
     </row>
@@ -3640,19 +3663,19 @@
       <c r="P14">
         <v>0.60552134273328895</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="5">
         <v>0.368207798405221</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="5">
         <v>0.37077006092352799</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="5">
         <v>0.40162066616186798</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="5">
         <v>0.30338400666537202</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="5">
         <v>0.43653988132146299</v>
       </c>
     </row>
@@ -3705,19 +3728,19 @@
       <c r="P15">
         <v>0.654742389620254</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="5">
         <v>0.54278337018241396</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="5">
         <v>0.516601496830007</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="5">
         <v>0.51503299483848997</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="5">
         <v>0.53491830256389405</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="5">
         <v>0.51662252992205304</v>
       </c>
     </row>
@@ -3770,19 +3793,19 @@
       <c r="P16">
         <v>0.91866215602618495</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="5">
         <v>0.82557601870369901</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="5">
         <v>0.81484069419298699</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="5">
         <v>0.81834345653901297</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="5">
         <v>0.81607856484351604</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="5">
         <v>0.81510192994570696</v>
       </c>
     </row>
@@ -3835,19 +3858,19 @@
       <c r="P17">
         <v>0.88143585861497498</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="5">
         <v>0.47328098901142102</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="5">
         <v>0.48646163445296098</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="5">
         <v>0.469899756407193</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="5">
         <v>0.47317205145831298</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="5">
         <v>0.47978211148025102</v>
       </c>
     </row>
@@ -3900,19 +3923,19 @@
       <c r="P18">
         <v>0.77335523941714501</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="5">
         <v>0.44681392802775499</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="5">
         <v>0.445912045037061</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="5">
         <v>0.44555366776910299</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="5">
         <v>0.44203792349187199</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="5">
         <v>0.44224839642376701</v>
       </c>
     </row>
@@ -3965,19 +3988,19 @@
       <c r="P19">
         <v>0.84225677326039505</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="5">
         <v>0.67107732059814795</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="5">
         <v>0.57819161761690196</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="5">
         <v>0.70766864704400101</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="5">
         <v>0.55511500745457498</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="5">
         <v>0.67139581516181202</v>
       </c>
     </row>
@@ -4030,19 +4053,19 @@
       <c r="P20">
         <v>0.543301521112867</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="5">
         <v>0.391196773980654</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="5">
         <v>0.394531377491255</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="5">
         <v>0.43069337557294901</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="5">
         <v>0.40151525718158299</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="5">
         <v>0.42157551064573601</v>
       </c>
     </row>
@@ -4095,19 +4118,19 @@
       <c r="P21">
         <v>0.48094397061624899</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="5">
         <v>0.42388591137533199</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="5">
         <v>0.41270265714696502</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="5">
         <v>0.41449738010207199</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="5">
         <v>0.41567852575281899</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="5">
         <v>0.42118713251066198</v>
       </c>
     </row>
@@ -4115,701 +4138,571 @@
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>0.92104873953440503</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>0.94331731524586004</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>0.93214935884945704</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>0.91808180724214805</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>0.94139186567493005</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>0.91675539279817098</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>0.92041550355439805</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>0.91754781635802296</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="3">
         <v>0.91457995058380503</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="3">
         <v>0.90887705408372699</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="3">
         <v>0.87052974979963005</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="3">
         <v>0.81752233783834205</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="3">
         <v>0.84362879591792705</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="3">
         <v>0.81545564777964097</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="3">
         <v>0.87036857989863903</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="6">
         <v>0.87314185265482402</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="6">
         <v>0.83658740931512598</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="4">
         <v>0.85550727622887002</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="6">
         <v>0.82232332260591501</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="6">
         <v>0.89476447229331102</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24">
-        <v>0.53737565259993703</v>
-      </c>
-      <c r="C24">
-        <v>0.55028710224474198</v>
-      </c>
-      <c r="D24">
-        <v>0.55554956781599996</v>
-      </c>
-      <c r="E24">
-        <v>0.53311628308014503</v>
-      </c>
-      <c r="F24">
-        <v>0.55327467237538197</v>
-      </c>
-      <c r="G24">
-        <v>0.74301488671953997</v>
-      </c>
-      <c r="H24">
-        <v>0.74688408672325501</v>
-      </c>
-      <c r="I24">
-        <v>0.74779829348982596</v>
-      </c>
-      <c r="J24">
-        <v>0.74659231404260795</v>
-      </c>
-      <c r="K24">
-        <v>0.73902185284579702</v>
-      </c>
-      <c r="L24">
-        <v>0.70980508120430097</v>
-      </c>
-      <c r="M24">
-        <v>0.67647965229154094</v>
-      </c>
-      <c r="N24">
-        <v>0.69533534134478703</v>
-      </c>
-      <c r="O24">
-        <v>0.67163413369019398</v>
-      </c>
-      <c r="P24">
-        <v>0.69532553017750798</v>
-      </c>
-      <c r="Q24">
-        <v>0.49962296743253898</v>
-      </c>
-      <c r="R24">
-        <v>0.48744731105626199</v>
-      </c>
-      <c r="S24">
-        <v>0.508600153945589</v>
-      </c>
-      <c r="T24">
-        <v>0.47442401766924602</v>
-      </c>
-      <c r="U24">
-        <v>0.51101197313632796</v>
+        <v>15</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.3629119386847299</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1.39601287161724</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.35815482407064</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1.3632043706411501</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1.3856276839111501</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1.06812343308003</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1.0714450500488999</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1.0647378575170501</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1.0600397668621699</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1.0564502160656499</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1.00983950081094</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.93824032245512201</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0.97098181952780604</v>
+      </c>
+      <c r="O24" s="3">
+        <v>0.939043825758205</v>
+      </c>
+      <c r="P24" s="3">
+        <v>1.0247625031765399</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>1.3104080722199301</v>
+      </c>
+      <c r="R24" s="6">
+        <v>1.2391321111015301</v>
+      </c>
+      <c r="S24" s="4">
+        <v>1.24875209984569</v>
+      </c>
+      <c r="T24" s="6">
+        <v>1.2267909534614201</v>
+      </c>
+      <c r="U24" s="6">
+        <v>1.34473879964773</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25">
-        <v>0.58263150281752996</v>
-      </c>
-      <c r="C25">
-        <v>0.60976539997009804</v>
-      </c>
-      <c r="D25">
-        <v>0.60600700717474298</v>
-      </c>
-      <c r="E25">
-        <v>0.59164986106829798</v>
-      </c>
-      <c r="F25">
-        <v>0.59837120428006396</v>
-      </c>
-      <c r="G25">
-        <v>0.743900470589408</v>
-      </c>
-      <c r="H25">
-        <v>0.75237332661060796</v>
-      </c>
-      <c r="I25">
-        <v>0.74668771230041298</v>
-      </c>
-      <c r="J25">
-        <v>0.74662641848148203</v>
-      </c>
-      <c r="K25">
-        <v>0.73854134837664698</v>
-      </c>
-      <c r="L25">
-        <v>0.71608078894291705</v>
-      </c>
-      <c r="M25">
-        <v>0.67939255242618501</v>
-      </c>
-      <c r="N25">
-        <v>0.69780618666710204</v>
-      </c>
-      <c r="O25">
-        <v>0.67500367467299605</v>
-      </c>
-      <c r="P25">
-        <v>0.70608409009127704</v>
-      </c>
-      <c r="Q25">
-        <v>0.54499942283793401</v>
-      </c>
-      <c r="R25">
-        <v>0.54205147392455799</v>
-      </c>
-      <c r="S25">
-        <v>0.55828544663425295</v>
-      </c>
-      <c r="T25">
-        <v>0.52844108770627096</v>
-      </c>
-      <c r="U25">
-        <v>0.55792710605370599</v>
+        <v>13</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.53737565259993703</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.55028710224474198</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.55554956781599996</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.53311628308014503</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.55327467237538197</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.74301488671953997</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.74688408672325501</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.74779829348982596</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.74659231404260795</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.73902185284579702</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.70980508120430097</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.67647965229154094</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0.69533534134478703</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0.67163413369019398</v>
+      </c>
+      <c r="P25" s="3">
+        <v>0.69532553017750798</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>0.49962296743253898</v>
+      </c>
+      <c r="R25" s="6">
+        <v>0.48744731105626199</v>
+      </c>
+      <c r="S25" s="4">
+        <v>0.508600153945589</v>
+      </c>
+      <c r="T25" s="6">
+        <v>0.47442401766924602</v>
+      </c>
+      <c r="U25" s="6">
+        <v>0.51101197313632796</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26">
-        <v>1.3629119386847299</v>
-      </c>
-      <c r="C26">
-        <v>1.39601287161724</v>
-      </c>
-      <c r="D26">
-        <v>1.35815482407064</v>
-      </c>
-      <c r="E26">
-        <v>1.3632043706411501</v>
-      </c>
-      <c r="F26">
-        <v>1.3856276839111501</v>
-      </c>
-      <c r="G26">
-        <v>1.06812343308003</v>
-      </c>
-      <c r="H26">
-        <v>1.0714450500488999</v>
-      </c>
-      <c r="I26">
-        <v>1.0647378575170501</v>
-      </c>
-      <c r="J26">
-        <v>1.0600397668621699</v>
-      </c>
-      <c r="K26">
-        <v>1.0564502160656499</v>
-      </c>
-      <c r="L26">
-        <v>1.00983950081094</v>
-      </c>
-      <c r="M26">
-        <v>0.93824032245512201</v>
-      </c>
-      <c r="N26">
-        <v>0.97098181952780604</v>
-      </c>
-      <c r="O26">
-        <v>0.939043825758205</v>
-      </c>
-      <c r="P26">
-        <v>1.0247625031765399</v>
-      </c>
-      <c r="Q26">
-        <v>1.3104080722199301</v>
-      </c>
-      <c r="R26">
-        <v>1.2391321111015301</v>
-      </c>
-      <c r="S26">
-        <v>1.24875209984569</v>
-      </c>
-      <c r="T26">
-        <v>1.2267909534614201</v>
-      </c>
-      <c r="U26">
-        <v>1.34473879964773</v>
+        <v>10</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1.18403729405432</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1.1971574817806101</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1.1829789559494499</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1.1326359329331199</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1.22185728744025</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1.1079002800286899</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1.1047346590978999</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1.10514707205036</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1.1031873527676701</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1.0977816860480301</v>
+      </c>
+      <c r="L26" s="3">
+        <v>1.01970287757066</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.920892360538626</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0.97243841705216705</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0.92127486123802904</v>
+      </c>
+      <c r="P26" s="3">
+        <v>1.0310167236707399</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>1.1160026422215801</v>
+      </c>
+      <c r="R26" s="6">
+        <v>1.0103909582970401</v>
+      </c>
+      <c r="S26" s="4">
+        <v>1.0593630977442801</v>
+      </c>
+      <c r="T26" s="6">
+        <v>0.980482950006061</v>
+      </c>
+      <c r="U26" s="6">
+        <v>1.16924075879523</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27">
-        <v>1.18403729405432</v>
-      </c>
-      <c r="C27">
-        <v>1.1971574817806101</v>
-      </c>
-      <c r="D27">
-        <v>1.1829789559494499</v>
-      </c>
-      <c r="E27">
-        <v>1.1326359329331199</v>
-      </c>
-      <c r="F27">
-        <v>1.22185728744025</v>
-      </c>
-      <c r="G27">
-        <v>1.1079002800286899</v>
-      </c>
-      <c r="H27">
-        <v>1.1047346590978999</v>
-      </c>
-      <c r="I27">
-        <v>1.10514707205036</v>
-      </c>
-      <c r="J27">
-        <v>1.1031873527676701</v>
-      </c>
-      <c r="K27">
-        <v>1.0977816860480301</v>
-      </c>
-      <c r="L27">
-        <v>1.01970287757066</v>
-      </c>
-      <c r="M27">
-        <v>0.920892360538626</v>
-      </c>
-      <c r="N27">
-        <v>0.97243841705216705</v>
-      </c>
-      <c r="O27">
-        <v>0.92127486123802904</v>
-      </c>
-      <c r="P27">
-        <v>1.0310167236707399</v>
-      </c>
-      <c r="Q27">
-        <v>1.1160026422215801</v>
-      </c>
-      <c r="R27">
-        <v>1.0103909582970401</v>
-      </c>
-      <c r="S27">
-        <v>1.0593630977442801</v>
-      </c>
-      <c r="T27">
-        <v>0.980482950006061</v>
-      </c>
-      <c r="U27">
-        <v>1.16924075879523</v>
+        <v>11</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.83217399687840998</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.837581349343829</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.83354706755545804</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.835414742320299</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.83841251630688896</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.80966290496209103</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.81544526681638996</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.815745831884085</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.81062565468690995</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.80623919025749002</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.79710259268663397</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.78825506634900899</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0.78676356987818297</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0.78150336083029204</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0.78237527234194204</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>0.80484733813403597</v>
+      </c>
+      <c r="R27" s="6">
+        <v>0.79585249130310898</v>
+      </c>
+      <c r="S27" s="4">
+        <v>0.79014097259287397</v>
+      </c>
+      <c r="T27" s="6">
+        <v>0.79221400987917701</v>
+      </c>
+      <c r="U27" s="6">
+        <v>0.79507931698374501</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28">
-        <v>0.83217399687840998</v>
-      </c>
-      <c r="C28">
-        <v>0.837581349343829</v>
-      </c>
-      <c r="D28">
-        <v>0.83354706755545804</v>
-      </c>
-      <c r="E28">
-        <v>0.835414742320299</v>
-      </c>
-      <c r="F28">
-        <v>0.83841251630688896</v>
-      </c>
-      <c r="G28">
-        <v>0.80966290496209103</v>
-      </c>
-      <c r="H28">
-        <v>0.81544526681638996</v>
-      </c>
-      <c r="I28">
-        <v>0.815745831884085</v>
-      </c>
-      <c r="J28">
-        <v>0.81062565468690995</v>
-      </c>
-      <c r="K28">
-        <v>0.80623919025749002</v>
-      </c>
-      <c r="L28">
-        <v>0.79710259268663397</v>
-      </c>
-      <c r="M28">
-        <v>0.78825506634900899</v>
-      </c>
-      <c r="N28">
-        <v>0.78676356987818297</v>
-      </c>
-      <c r="O28">
-        <v>0.78150336083029204</v>
-      </c>
-      <c r="P28">
-        <v>0.78237527234194204</v>
-      </c>
-      <c r="Q28">
-        <v>0.80484733813403597</v>
-      </c>
-      <c r="R28">
-        <v>0.79585249130310898</v>
-      </c>
-      <c r="S28">
-        <v>0.79014097259287397</v>
-      </c>
-      <c r="T28">
-        <v>0.79221400987917701</v>
-      </c>
-      <c r="U28">
-        <v>0.79507931698374501</v>
+        <v>16</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.39872070250257002</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.442681133624235</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.42443791152763899</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.38543270886326703</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.43116875177831598</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.52063443382566199</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.52533012273102497</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.52417793439785798</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.51992702661818702</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.52079422541990505</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.50355704828713199</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.49237693609876398</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0.50630736725546199</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0.48134411808185001</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0.50497869900475201</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>0.37723666371029202</v>
+      </c>
+      <c r="R28" s="6">
+        <v>0.38009785128266199</v>
+      </c>
+      <c r="S28" s="4">
+        <v>0.406722639435945</v>
+      </c>
+      <c r="T28" s="6">
+        <v>0.33937233037051501</v>
+      </c>
+      <c r="U28" s="6">
+        <v>0.421342440810832</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29">
-        <v>0.887740570940031</v>
-      </c>
-      <c r="C29">
-        <v>0.91171315241184703</v>
-      </c>
-      <c r="D29">
-        <v>0.896966991358076</v>
-      </c>
-      <c r="E29">
-        <v>0.89111122100209705</v>
-      </c>
-      <c r="F29">
-        <v>0.90295376830179097</v>
-      </c>
-      <c r="G29">
-        <v>0.86763973937613403</v>
-      </c>
-      <c r="H29">
-        <v>0.87300395031802303</v>
-      </c>
-      <c r="I29">
-        <v>0.86796143186625996</v>
-      </c>
-      <c r="J29">
-        <v>0.86608629246997004</v>
-      </c>
-      <c r="K29">
-        <v>0.86001293032333104</v>
-      </c>
-      <c r="L29">
-        <v>0.83599433304526505</v>
-      </c>
-      <c r="M29">
-        <v>0.78914470067724596</v>
-      </c>
-      <c r="N29">
-        <v>0.80962021225958503</v>
-      </c>
-      <c r="O29">
-        <v>0.78750993650529699</v>
-      </c>
-      <c r="P29">
-        <v>0.83378145123654102</v>
-      </c>
-      <c r="Q29">
-        <v>0.84678870681227003</v>
-      </c>
-      <c r="R29">
-        <v>0.81714481499151004</v>
-      </c>
-      <c r="S29">
-        <v>0.83262610944258897</v>
-      </c>
-      <c r="T29">
-        <v>0.80514136414751203</v>
-      </c>
-      <c r="U29">
-        <v>0.86223111334772795</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30">
-        <v>0.39872070250257002</v>
-      </c>
-      <c r="C30">
-        <v>0.442681133624235</v>
-      </c>
-      <c r="D30">
-        <v>0.42443791152763899</v>
-      </c>
-      <c r="E30">
-        <v>0.38543270886326703</v>
-      </c>
-      <c r="F30">
-        <v>0.43116875177831598</v>
-      </c>
-      <c r="G30">
-        <v>0.52063443382566199</v>
-      </c>
-      <c r="H30">
-        <v>0.52533012273102497</v>
-      </c>
-      <c r="I30">
-        <v>0.52417793439785798</v>
-      </c>
-      <c r="J30">
-        <v>0.51992702661818702</v>
-      </c>
-      <c r="K30">
-        <v>0.52079422541990505</v>
-      </c>
-      <c r="L30">
-        <v>0.50355704828713199</v>
-      </c>
-      <c r="M30">
-        <v>0.49237693609876398</v>
-      </c>
-      <c r="N30">
-        <v>0.50630736725546199</v>
-      </c>
-      <c r="O30">
-        <v>0.48134411808185001</v>
-      </c>
-      <c r="P30">
-        <v>0.50497869900475201</v>
-      </c>
-      <c r="Q30">
-        <v>0.37723666371029202</v>
-      </c>
-      <c r="R30">
-        <v>0.38009785128266199</v>
-      </c>
-      <c r="S30">
-        <v>0.406722639435945</v>
-      </c>
-      <c r="T30">
-        <v>0.33937233037051501</v>
-      </c>
-      <c r="U30">
-        <v>0.421342440810832</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B31">
+      <c r="B29" s="3">
         <v>2.28895132226085</v>
       </c>
-      <c r="C31">
+      <c r="C29" s="3">
         <v>2.1817644912906902</v>
       </c>
-      <c r="D31">
+      <c r="D29" s="3">
         <v>2.2313923569536902</v>
       </c>
-      <c r="E31">
+      <c r="E29" s="3">
         <v>2.2159586181722699</v>
       </c>
-      <c r="F31">
+      <c r="F29" s="3">
         <v>2.2417727417528801</v>
       </c>
-      <c r="G31">
+      <c r="G29" s="3">
         <v>2.0216418589084202</v>
       </c>
-      <c r="H31">
+      <c r="H29" s="3">
         <v>2.0150010527196498</v>
       </c>
-      <c r="I31">
+      <c r="I29" s="3">
         <v>2.02399620404322</v>
       </c>
-      <c r="J31">
+      <c r="J29" s="3">
         <v>2.0169222540217602</v>
       </c>
-      <c r="K31">
+      <c r="K29" s="3">
         <v>2.0192212528422999</v>
       </c>
-      <c r="L31">
+      <c r="L29" s="3">
         <v>1.79090913664421</v>
       </c>
-      <c r="M31">
+      <c r="M29" s="3">
         <v>1.65378617455639</v>
       </c>
-      <c r="N31">
+      <c r="N29" s="3">
         <v>1.6914686108827</v>
       </c>
-      <c r="O31">
+      <c r="O29" s="3">
         <v>1.70271862725685</v>
       </c>
-      <c r="P31">
+      <c r="P29" s="3">
         <v>1.79224212151579</v>
       </c>
-      <c r="Q31">
+      <c r="Q29" s="6">
         <v>2.05068372355325</v>
       </c>
-      <c r="R31">
+      <c r="R29" s="6">
         <v>1.8820899859168601</v>
       </c>
-      <c r="S31">
+      <c r="S29" s="4">
         <v>1.9243509711423401</v>
       </c>
-      <c r="T31">
+      <c r="T29" s="6">
         <v>1.9195673943423299</v>
       </c>
-      <c r="U31">
+      <c r="U29" s="6">
         <v>1.99183873738692</v>
       </c>
     </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <f>G23</f>
+        <v>0.91675539279817098</v>
+      </c>
+      <c r="C33">
+        <f>H23</f>
+        <v>0.92041550355439805</v>
+      </c>
+      <c r="D33">
+        <f>I23</f>
+        <v>0.91754781635802296</v>
+      </c>
+      <c r="E33">
+        <f>J23</f>
+        <v>0.91457995058380503</v>
+      </c>
+      <c r="F33">
+        <f>K23</f>
+        <v>0.90887705408372699</v>
+      </c>
+    </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" t="s">
-        <v>4</v>
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <f>B23</f>
+        <v>0.92104873953440503</v>
+      </c>
+      <c r="C34">
+        <f>C23</f>
+        <v>0.94331731524586004</v>
+      </c>
+      <c r="D34">
+        <f>D23</f>
+        <v>0.93214935884945704</v>
+      </c>
+      <c r="E34">
+        <f>E23</f>
+        <v>0.91808180724214805</v>
+      </c>
+      <c r="F34">
+        <f>F23</f>
+        <v>0.94139186567493005</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B35">
-        <f>G23</f>
-        <v>0.91675539279817098</v>
+        <f>L23</f>
+        <v>0.87052974979963005</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:F35" si="0">H23</f>
-        <v>0.92041550355439805</v>
+        <f>M23</f>
+        <v>0.81752233783834205</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
-        <v>0.91754781635802296</v>
+        <f>N23</f>
+        <v>0.84362879591792705</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
-        <v>0.91457995058380503</v>
+        <f>O23</f>
+        <v>0.81545564777964097</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
-        <v>0.90887705408372699</v>
+        <f>P23</f>
+        <v>0.87036857989863903</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B36">
-        <f>B23</f>
-        <v>0.92104873953440503</v>
-      </c>
-      <c r="C36">
-        <f t="shared" ref="C36:F36" si="1">C23</f>
-        <v>0.94331731524586004</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="1"/>
-        <v>0.93214935884945704</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="1"/>
-        <v>0.91808180724214805</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="1"/>
-        <v>0.94139186567493005</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37">
-        <f>L23</f>
-        <v>0.87052974979963005</v>
-      </c>
-      <c r="C37">
-        <f t="shared" ref="C37:F37" si="2">M23</f>
-        <v>0.81752233783834205</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="2"/>
-        <v>0.84362879591792705</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="2"/>
-        <v>0.81545564777964097</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="2"/>
-        <v>0.87036857989863903</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38">
         <f>Q23</f>
         <v>0.87314185265482402</v>
       </c>
-      <c r="C38">
-        <f t="shared" ref="C38:F38" si="3">R23</f>
+      <c r="C36">
+        <f>R23</f>
         <v>0.83658740931512598</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="3"/>
+      <c r="D36">
+        <f>S23</f>
         <v>0.85550727622887002</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="3"/>
+      <c r="E36">
+        <f>T23</f>
         <v>0.82232332260591501</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="3"/>
+      <c r="F36">
+        <f>U23</f>
         <v>0.89476447229331102</v>
       </c>
     </row>
@@ -4823,8 +4716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14AFAA2-6A31-4AF8-898F-B86E5B8F3F99}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8040,4 +7933,2384 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AB9A19-C1A5-4634-86C6-32934B15812C}">
+  <dimension ref="A1:U9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.92104873953440503</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.94331731524586004</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.93214935884945704</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.91808180724214805</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.94139186567493005</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.91675539279817098</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.92041550355439805</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.91754781635802296</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.91457995058380503</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.90887705408372699</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.87052974979963005</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.81752233783834205</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.84362879591792705</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0.81545564777964097</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.87036857989863903</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0.87314185265482402</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0.83658740931512598</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0.85550727622887002</v>
+      </c>
+      <c r="T3" s="6">
+        <v>0.82232332260591501</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0.89476447229331102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.3629119386847299</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.39601287161724</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.35815482407064</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.3632043706411501</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.3856276839111501</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.06812343308003</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1.0714450500488999</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.0647378575170501</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.0600397668621699</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.0564502160656499</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1.00983950081094</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.93824032245512201</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.97098181952780604</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.939043825758205</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1.0247625031765399</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1.3104080722199301</v>
+      </c>
+      <c r="R4" s="6">
+        <v>1.2391321111015301</v>
+      </c>
+      <c r="S4" s="4">
+        <v>1.24875209984569</v>
+      </c>
+      <c r="T4" s="6">
+        <v>1.2267909534614201</v>
+      </c>
+      <c r="U4" s="6">
+        <v>1.34473879964773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.53737565259993703</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.55028710224474198</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.55554956781599996</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.53311628308014503</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.55327467237538197</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.74301488671953997</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.74688408672325501</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.74779829348982596</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.74659231404260795</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.73902185284579702</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.70980508120430097</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.67647965229154094</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.69533534134478703</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.67163413369019398</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.69532553017750798</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0.49962296743253898</v>
+      </c>
+      <c r="R5" s="6">
+        <v>0.48744731105626199</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0.508600153945589</v>
+      </c>
+      <c r="T5" s="6">
+        <v>0.47442401766924602</v>
+      </c>
+      <c r="U5" s="6">
+        <v>0.51101197313632796</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.18403729405432</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.1971574817806101</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.1829789559494499</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.1326359329331199</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.22185728744025</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.1079002800286899</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1.1047346590978999</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.10514707205036</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.1031873527676701</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.0977816860480301</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1.01970287757066</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.920892360538626</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.97243841705216705</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.92127486123802904</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1.0310167236707399</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1.1160026422215801</v>
+      </c>
+      <c r="R6" s="6">
+        <v>1.0103909582970401</v>
+      </c>
+      <c r="S6" s="4">
+        <v>1.0593630977442801</v>
+      </c>
+      <c r="T6" s="6">
+        <v>0.980482950006061</v>
+      </c>
+      <c r="U6" s="6">
+        <v>1.16924075879523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.83217399687840998</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.837581349343829</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.83354706755545804</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.835414742320299</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.83841251630688896</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.80966290496209103</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.81544526681638996</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.815745831884085</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.81062565468690995</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.80623919025749002</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.79710259268663397</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.78825506634900899</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.78676356987818297</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.78150336083029204</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0.78237527234194204</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0.80484733813403597</v>
+      </c>
+      <c r="R7" s="6">
+        <v>0.79585249130310898</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0.79014097259287397</v>
+      </c>
+      <c r="T7" s="6">
+        <v>0.79221400987917701</v>
+      </c>
+      <c r="U7" s="6">
+        <v>0.79507931698374501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.39872070250257002</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.442681133624235</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.42443791152763899</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.38543270886326703</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.43116875177831598</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.52063443382566199</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.52533012273102497</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.52417793439785798</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.51992702661818702</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.52079422541990505</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.50355704828713199</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.49237693609876398</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.50630736725546199</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.48134411808185001</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.50497869900475201</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>0.37723666371029202</v>
+      </c>
+      <c r="R8" s="6">
+        <v>0.38009785128266199</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0.406722639435945</v>
+      </c>
+      <c r="T8" s="6">
+        <v>0.33937233037051501</v>
+      </c>
+      <c r="U8" s="6">
+        <v>0.421342440810832</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.28895132226085</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.1817644912906902</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.2313923569536902</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2.2159586181722699</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.2417727417528801</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.0216418589084202</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2.0150010527196498</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2.02399620404322</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2.0169222540217602</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2.0192212528422999</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1.79090913664421</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1.65378617455639</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1.6914686108827</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1.70271862725685</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1.79224212151579</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>2.05068372355325</v>
+      </c>
+      <c r="R9" s="6">
+        <v>1.8820899859168601</v>
+      </c>
+      <c r="S9" s="4">
+        <v>1.9243509711423401</v>
+      </c>
+      <c r="T9" s="6">
+        <v>1.9195673943423299</v>
+      </c>
+      <c r="U9" s="6">
+        <v>1.99183873738692</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9598D015-DFDD-42D8-9B86-66EC211E3749}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.92104873953440503</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.39872070250257002</v>
+      </c>
+      <c r="E2" s="6">
+        <v>2.28895132226085</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1.3629119386847299</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.53737565259993703</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1.18403729405432</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.83217399687840998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.94331731524586004</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.442681133624235</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2.1817644912906902</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.39601287161724</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.55028710224474198</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.1971574817806101</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.837581349343829</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.93214935884945704</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.42443791152763899</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2.2313923569536902</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1.35815482407064</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.55554956781599996</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1.1829789559494499</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.83354706755545804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.91808180724214805</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.38543270886326703</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2.2159586181722699</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.3632043706411501</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.53311628308014503</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1.1326359329331199</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.835414742320299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.94139186567493005</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.43116875177831598</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2.2417727417528801</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1.3856276839111501</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.55327467237538197</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1.22185728744025</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.83841251630688896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.91675539279817098</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.52063443382566199</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.0216418589084202</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.06812343308003</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.74301488671953997</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.1079002800286899</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.80966290496209103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.92041550355439805</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.52533012273102497</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2.0150010527196498</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.0714450500488999</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.74688408672325501</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.1047346590978999</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.81544526681638996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.91754781635802296</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.52417793439785798</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2.02399620404322</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.0647378575170501</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.74779829348982596</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1.10514707205036</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.815745831884085</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.91457995058380503</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.51992702661818702</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.0169222540217602</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.0600397668621699</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.74659231404260795</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1.1031873527676701</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.81062565468690995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.90887705408372699</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.52079422541990505</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.0192212528422999</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.0564502160656499</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.73902185284579702</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1.0977816860480301</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.80623919025749002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.87052974979963005</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.50355704828713199</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.79090913664421</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1.00983950081094</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.70980508120430097</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1.01970287757066</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.79710259268663397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.81752233783834205</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.49237693609876398</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.65378617455639</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.93824032245512201</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.67647965229154094</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.920892360538626</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.78825506634900899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.84362879591792705</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.50630736725546199</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.6914686108827</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.97098181952780604</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.69533534134478703</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.97243841705216705</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.78676356987818297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.81545564777964097</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.48134411808185001</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.70271862725685</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.939043825758205</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.67163413369019398</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.92127486123802904</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.78150336083029204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.87036857989863903</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.50497869900475201</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.79224212151579</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.0247625031765399</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.69532553017750798</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.0310167236707399</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.78237527234194204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.87314185265482402</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.37723666371029202</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2.05068372355325</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1.3104080722199301</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.49962296743253898</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1.1160026422215801</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.80484733813403597</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.83658740931512598</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.38009785128266199</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1.8820899859168601</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1.2391321111015301</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.48744731105626199</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1.0103909582970401</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.79585249130310898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.85550727622887002</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.406722639435945</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.9243509711423401</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1.24875209984569</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.508600153945589</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1.0593630977442801</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.79014097259287397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.82232332260591501</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.33937233037051501</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.9195673943423299</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1.2267909534614201</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.47442401766924602</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.980482950006061</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.79221400987917701</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.89476447229331102</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.421342440810832</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1.99183873738692</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1.34473879964773</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.51101197313632796</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.16924075879523</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.79507931698374501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667C3666-C0EF-40D8-89E0-66A47AFC4467}">
+  <dimension ref="A1:U11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.94938044926493603</v>
+      </c>
+      <c r="C3">
+        <v>0.96806725218411305</v>
+      </c>
+      <c r="D3">
+        <v>0.95241108018071496</v>
+      </c>
+      <c r="E3">
+        <v>0.92356333586795802</v>
+      </c>
+      <c r="F3">
+        <v>0.97590381658999903</v>
+      </c>
+      <c r="G3">
+        <v>0.91838147908781798</v>
+      </c>
+      <c r="H3">
+        <v>0.92060335060746401</v>
+      </c>
+      <c r="I3">
+        <v>0.91944893040768105</v>
+      </c>
+      <c r="J3">
+        <v>0.92010276863599505</v>
+      </c>
+      <c r="K3">
+        <v>0.92311432519418801</v>
+      </c>
+      <c r="L3">
+        <v>0.844098009428909</v>
+      </c>
+      <c r="M3">
+        <v>0.78865257522550802</v>
+      </c>
+      <c r="N3">
+        <v>0.81148618980418197</v>
+      </c>
+      <c r="O3">
+        <v>0.78789417178358201</v>
+      </c>
+      <c r="P3">
+        <v>0.84987413595704298</v>
+      </c>
+      <c r="Q3">
+        <v>0.87871728456422604</v>
+      </c>
+      <c r="R3">
+        <v>0.82871449802539399</v>
+      </c>
+      <c r="S3">
+        <v>0.84391478498513695</v>
+      </c>
+      <c r="T3">
+        <v>0.79683122565895304</v>
+      </c>
+      <c r="U3">
+        <v>0.89962684726208397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0.68946204079215101</v>
+      </c>
+      <c r="C4">
+        <v>0.70914233879380295</v>
+      </c>
+      <c r="D4">
+        <v>0.70749585373886203</v>
+      </c>
+      <c r="E4">
+        <v>0.68190490526460401</v>
+      </c>
+      <c r="F4">
+        <v>0.71191789592425903</v>
+      </c>
+      <c r="G4">
+        <v>0.93492125105602197</v>
+      </c>
+      <c r="H4">
+        <v>0.93033737678638395</v>
+      </c>
+      <c r="I4">
+        <v>0.931498366548978</v>
+      </c>
+      <c r="J4">
+        <v>0.93339903632519505</v>
+      </c>
+      <c r="K4">
+        <v>0.93597275412247105</v>
+      </c>
+      <c r="L4">
+        <v>0.84553086578377701</v>
+      </c>
+      <c r="M4">
+        <v>0.80188025171210897</v>
+      </c>
+      <c r="N4">
+        <v>0.832744807636563</v>
+      </c>
+      <c r="O4">
+        <v>0.79742323501419798</v>
+      </c>
+      <c r="P4">
+        <v>0.85096094693292401</v>
+      </c>
+      <c r="Q4">
+        <v>0.62222999364878295</v>
+      </c>
+      <c r="R4">
+        <v>0.59751924443922899</v>
+      </c>
+      <c r="S4">
+        <v>0.61838601448478203</v>
+      </c>
+      <c r="T4">
+        <v>0.57805352347486105</v>
+      </c>
+      <c r="U4">
+        <v>0.63639443914441396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.69607733959112095</v>
+      </c>
+      <c r="C5">
+        <v>0.72632214972554998</v>
+      </c>
+      <c r="D5">
+        <v>0.71823555373474601</v>
+      </c>
+      <c r="E5">
+        <v>0.69564614861168095</v>
+      </c>
+      <c r="F5">
+        <v>0.71752174841417604</v>
+      </c>
+      <c r="G5">
+        <v>0.86931438193713095</v>
+      </c>
+      <c r="H5">
+        <v>0.86895724954963005</v>
+      </c>
+      <c r="I5">
+        <v>0.869772920010355</v>
+      </c>
+      <c r="J5">
+        <v>0.870159060483226</v>
+      </c>
+      <c r="K5">
+        <v>0.87321653436214597</v>
+      </c>
+      <c r="L5">
+        <v>0.79355816662637302</v>
+      </c>
+      <c r="M5">
+        <v>0.75080788618222105</v>
+      </c>
+      <c r="N5">
+        <v>0.77756952786879296</v>
+      </c>
+      <c r="O5">
+        <v>0.74634716014804503</v>
+      </c>
+      <c r="P5">
+        <v>0.80005148312885999</v>
+      </c>
+      <c r="Q5">
+        <v>0.63094563553889005</v>
+      </c>
+      <c r="R5">
+        <v>0.61524074492740599</v>
+      </c>
+      <c r="S5">
+        <v>0.63330915371582097</v>
+      </c>
+      <c r="T5">
+        <v>0.59330825195479797</v>
+      </c>
+      <c r="U5">
+        <v>0.64766603948340895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>1.19806457885439</v>
+      </c>
+      <c r="C6">
+        <v>1.21398276425677</v>
+      </c>
+      <c r="D6">
+        <v>1.1822674729557401</v>
+      </c>
+      <c r="E6">
+        <v>1.1515417267649599</v>
+      </c>
+      <c r="F6">
+        <v>1.2275147802923401</v>
+      </c>
+      <c r="G6">
+        <v>0.906536637192074</v>
+      </c>
+      <c r="H6">
+        <v>0.91358808936346103</v>
+      </c>
+      <c r="I6">
+        <v>0.91078371902221</v>
+      </c>
+      <c r="J6">
+        <v>0.91055187585313002</v>
+      </c>
+      <c r="K6">
+        <v>0.91387383315537196</v>
+      </c>
+      <c r="L6">
+        <v>0.84305745743516303</v>
+      </c>
+      <c r="M6">
+        <v>0.77916970562854104</v>
+      </c>
+      <c r="N6">
+        <v>0.79636704249246804</v>
+      </c>
+      <c r="O6">
+        <v>0.78103554399129005</v>
+      </c>
+      <c r="P6">
+        <v>0.84908459989543905</v>
+      </c>
+      <c r="Q6">
+        <v>1.12944753467328</v>
+      </c>
+      <c r="R6">
+        <v>1.0512747613281399</v>
+      </c>
+      <c r="S6">
+        <v>1.0580561875828101</v>
+      </c>
+      <c r="T6">
+        <v>1.0063450632643101</v>
+      </c>
+      <c r="U6">
+        <v>1.157171431092</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1.0535592389272299</v>
+      </c>
+      <c r="C7">
+        <v>1.07346539838855</v>
+      </c>
+      <c r="D7">
+        <v>1.03933886945119</v>
+      </c>
+      <c r="E7">
+        <v>0.99430688446874205</v>
+      </c>
+      <c r="F7">
+        <v>1.09877087039096</v>
+      </c>
+      <c r="G7">
+        <v>0.99410333695618902</v>
+      </c>
+      <c r="H7">
+        <v>0.99987559747397003</v>
+      </c>
+      <c r="I7">
+        <v>0.99720275458268604</v>
+      </c>
+      <c r="J7">
+        <v>0.99810319634049005</v>
+      </c>
+      <c r="K7">
+        <v>1.00131991344468</v>
+      </c>
+      <c r="L7">
+        <v>0.89213048172484799</v>
+      </c>
+      <c r="M7">
+        <v>0.80074820914285005</v>
+      </c>
+      <c r="N7">
+        <v>0.82964182947704501</v>
+      </c>
+      <c r="O7">
+        <v>0.80411340448469004</v>
+      </c>
+      <c r="P7">
+        <v>0.89771393609477601</v>
+      </c>
+      <c r="Q7">
+        <v>0.97264420435576004</v>
+      </c>
+      <c r="R7">
+        <v>0.88739575805566295</v>
+      </c>
+      <c r="S7">
+        <v>0.90409079267961401</v>
+      </c>
+      <c r="T7">
+        <v>0.83209703714222905</v>
+      </c>
+      <c r="U7">
+        <v>1.0122325765665099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.98263382698266799</v>
+      </c>
+      <c r="C8">
+        <v>0.98352034489042806</v>
+      </c>
+      <c r="D8">
+        <v>0.98338900374646299</v>
+      </c>
+      <c r="E8">
+        <v>0.97936591663535499</v>
+      </c>
+      <c r="F8">
+        <v>0.98294114195662796</v>
+      </c>
+      <c r="G8">
+        <v>0.86665940010183795</v>
+      </c>
+      <c r="H8">
+        <v>0.86289108809422299</v>
+      </c>
+      <c r="I8">
+        <v>0.86702397293400602</v>
+      </c>
+      <c r="J8">
+        <v>0.86380162566831797</v>
+      </c>
+      <c r="K8">
+        <v>0.86948090792118904</v>
+      </c>
+      <c r="L8">
+        <v>0.82264467425163601</v>
+      </c>
+      <c r="M8">
+        <v>0.80542915855659403</v>
+      </c>
+      <c r="N8">
+        <v>0.81893668045014201</v>
+      </c>
+      <c r="O8">
+        <v>0.79739374261979801</v>
+      </c>
+      <c r="P8">
+        <v>0.82664773470756203</v>
+      </c>
+      <c r="Q8">
+        <v>0.92267878493473998</v>
+      </c>
+      <c r="R8">
+        <v>0.89221485111820797</v>
+      </c>
+      <c r="S8">
+        <v>0.90341005742081903</v>
+      </c>
+      <c r="T8">
+        <v>0.88705164530442404</v>
+      </c>
+      <c r="U8">
+        <v>0.92126602484695297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>0.93658118854585404</v>
+      </c>
+      <c r="C9">
+        <v>0.95643837324263603</v>
+      </c>
+      <c r="D9">
+        <v>0.94068670846994296</v>
+      </c>
+      <c r="E9">
+        <v>0.91319588175597999</v>
+      </c>
+      <c r="F9">
+        <v>0.96129781915066903</v>
+      </c>
+      <c r="G9">
+        <v>0.89739829019355899</v>
+      </c>
+      <c r="H9">
+        <v>0.89825849053066198</v>
+      </c>
+      <c r="I9">
+        <v>0.89875389703339403</v>
+      </c>
+      <c r="J9">
+        <v>0.89914298231872103</v>
+      </c>
+      <c r="K9">
+        <v>0.90261855422648596</v>
+      </c>
+      <c r="L9">
+        <v>0.83105112641436196</v>
+      </c>
+      <c r="M9">
+        <v>0.77907992451272101</v>
+      </c>
+      <c r="N9">
+        <v>0.80382333150874297</v>
+      </c>
+      <c r="O9">
+        <v>0.77574325021085599</v>
+      </c>
+      <c r="P9">
+        <v>0.83862937228804102</v>
+      </c>
+      <c r="Q9">
+        <v>0.86816726441759096</v>
+      </c>
+      <c r="R9">
+        <v>0.82153958283989303</v>
+      </c>
+      <c r="S9">
+        <v>0.837574693015955</v>
+      </c>
+      <c r="T9">
+        <v>0.79172565760975699</v>
+      </c>
+      <c r="U9">
+        <v>0.888041167892342</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0.47464576410988901</v>
+      </c>
+      <c r="C10">
+        <v>0.52743138115515398</v>
+      </c>
+      <c r="D10">
+        <v>0.50102886537054503</v>
+      </c>
+      <c r="E10">
+        <v>0.44922172094044799</v>
+      </c>
+      <c r="F10">
+        <v>0.52626953500958495</v>
+      </c>
+      <c r="G10">
+        <v>0.56936240861509602</v>
+      </c>
+      <c r="H10">
+        <v>0.57558899594750101</v>
+      </c>
+      <c r="I10">
+        <v>0.56986926980484498</v>
+      </c>
+      <c r="J10">
+        <v>0.57310202809733402</v>
+      </c>
+      <c r="K10">
+        <v>0.58253846628119299</v>
+      </c>
+      <c r="L10">
+        <v>0.53794273470699705</v>
+      </c>
+      <c r="M10">
+        <v>0.50346072339661596</v>
+      </c>
+      <c r="N10">
+        <v>0.52354164926914304</v>
+      </c>
+      <c r="O10">
+        <v>0.49946679492152801</v>
+      </c>
+      <c r="P10">
+        <v>0.54738793345076897</v>
+      </c>
+      <c r="Q10">
+        <v>0.431956056225754</v>
+      </c>
+      <c r="R10">
+        <v>0.421814599845241</v>
+      </c>
+      <c r="S10">
+        <v>0.43050719390157899</v>
+      </c>
+      <c r="T10">
+        <v>0.36947966229346402</v>
+      </c>
+      <c r="U10">
+        <v>0.462330443789849</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1.8376877324457099</v>
+      </c>
+      <c r="C11">
+        <v>1.75657753028879</v>
+      </c>
+      <c r="D11">
+        <v>1.74584794369288</v>
+      </c>
+      <c r="E11">
+        <v>1.7694592891794501</v>
+      </c>
+      <c r="F11">
+        <v>1.8457748402988099</v>
+      </c>
+      <c r="G11">
+        <v>1.4997216931386701</v>
+      </c>
+      <c r="H11">
+        <v>1.4982714256765901</v>
+      </c>
+      <c r="I11">
+        <v>1.5029170180985501</v>
+      </c>
+      <c r="J11">
+        <v>1.50409238088298</v>
+      </c>
+      <c r="K11">
+        <v>1.4911484149510199</v>
+      </c>
+      <c r="L11">
+        <v>1.3583705087276201</v>
+      </c>
+      <c r="M11">
+        <v>1.17194285633846</v>
+      </c>
+      <c r="N11">
+        <v>1.1989974873493201</v>
+      </c>
+      <c r="O11">
+        <v>1.1662873773254101</v>
+      </c>
+      <c r="P11">
+        <v>1.3579021012793699</v>
+      </c>
+      <c r="Q11">
+        <v>1.7859718419858099</v>
+      </c>
+      <c r="R11">
+        <v>1.6777629192324399</v>
+      </c>
+      <c r="S11">
+        <v>1.6249454527950999</v>
+      </c>
+      <c r="T11">
+        <v>1.66486077320231</v>
+      </c>
+      <c r="U11">
+        <v>1.7989160598314899</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B308347-3BD9-4E0F-A30D-E3D62248BF99}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.94938044926493603</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.47464576410988901</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1.8376877324457099</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1.19806457885439</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.68946204079215101</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1.0535592389272299</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.98263382698266799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.96806725218411305</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.52743138115515398</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.75657753028879</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1.21398276425677</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.70914233879380295</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.07346539838855</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.98352034489042806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.95241108018071496</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.50102886537054503</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1.74584794369288</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1.1822674729557401</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.70749585373886203</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1.03933886945119</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.98338900374646299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.92356333586795802</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.44922172094044799</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.7694592891794501</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.1515417267649599</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.68190490526460401</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.99430688446874205</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.97936591663535499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.97590381658999903</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.52626953500958495</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1.8457748402988099</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1.2275147802923401</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.71191789592425903</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1.09877087039096</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.98294114195662796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.91838147908781798</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.56936240861509602</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.4997216931386701</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.906536637192074</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.93492125105602197</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.99410333695618902</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.86665940010183795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.92060335060746401</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.57558899594750101</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.4982714256765901</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.91358808936346103</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.93033737678638395</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.99987559747397003</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.86289108809422299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.91944893040768105</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.56986926980484498</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.5029170180985501</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.91078371902221</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.931498366548978</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.99720275458268604</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.86702397293400602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.92010276863599505</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.57310202809733402</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.50409238088298</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.91055187585313002</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.93339903632519505</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.99810319634049005</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.86380162566831797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.92311432519418801</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.58253846628119299</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.4911484149510199</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.91387383315537196</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.93597275412247105</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1.00131991344468</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.86948090792118904</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.844098009428909</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.53794273470699705</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.3583705087276201</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.84305745743516303</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.84553086578377701</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.89213048172484799</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.82264467425163601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.78865257522550802</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.50346072339661596</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.17194285633846</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.77916970562854104</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.80188025171210897</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.80074820914285005</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.80542915855659403</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.81148618980418197</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.52354164926914304</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.1989974873493201</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.79636704249246804</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.832744807636563</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.82964182947704501</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.81893668045014201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.78789417178358201</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.49946679492152801</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.1662873773254101</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.78103554399129005</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.79742323501419798</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.80411340448469004</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.79739374261979801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.84987413595704298</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.54738793345076897</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.3579021012793699</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.84908459989543905</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.85096094693292401</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.89771393609477601</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.82664773470756203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.87871728456422604</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.431956056225754</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1.7859718419858099</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1.12944753467328</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.62222999364878295</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.97264420435576004</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.92267878493473998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.82871449802539399</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.421814599845241</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1.6777629192324399</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1.0512747613281399</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.59751924443922899</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.88739575805566295</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.89221485111820797</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.84391478498513695</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.43050719390157899</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.6249454527950999</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1.0580561875828101</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.61838601448478203</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.90409079267961401</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.90341005742081903</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.79683122565895304</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.36947966229346402</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.66486077320231</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1.0063450632643101</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.57805352347486105</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.83209703714222905</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.88705164530442404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.89962684726208397</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.462330443789849</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1.7989160598314899</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1.157171431092</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.63639443914441396</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.0122325765665099</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.92126602484695297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>